<commit_message>
membuat upload data master
</commit_message>
<xml_diff>
--- a/panel/file-excel/template_data_agama.xlsx
+++ b/panel/file-excel/template_data_agama.xlsx
@@ -177,6 +177,9 @@
     <t>User Input</t>
   </si>
   <si>
+    <t>Id User</t>
+  </si>
+  <si>
     <t>A1</t>
   </si>
   <si>
@@ -190,9 +193,6 @@
   </si>
   <si>
     <t>Katholik</t>
-  </si>
-  <si>
-    <t>Id User</t>
   </si>
 </sst>
 </file>
@@ -216,13 +216,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -266,14 +266,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,19 +554,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -575,148 +575,67 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3">
-        <v>44910</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="D3" s="4">
+        <v>44907</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44907</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>44911</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>